<commit_message>
Gen AI Question to answer mapping
</commit_message>
<xml_diff>
--- a/QPaperAnalyzerProject/QPaperAnalyzerApp/media/Excel_Files/Temp_QPapers/CST204_Regular_July_2021.xlsx
+++ b/QPaperAnalyzerProject/QPaperAnalyzerApp/media/Excel_Files/Temp_QPapers/CST204_Regular_July_2021.xlsx
@@ -382,10 +382,10 @@
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="44"/>

</xml_diff>